<commit_message>
Answer evaluation data in excel file
</commit_message>
<xml_diff>
--- a/data/Sample_data.xlsx
+++ b/data/Sample_data.xlsx
@@ -7,14 +7,26 @@
     <workbookView xWindow="360" yWindow="75" windowWidth="11355" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Q1" sheetId="2" r:id="rId2"/>
+    <sheet name="Q2" sheetId="3" r:id="rId3"/>
+    <sheet name="Q3" sheetId="4" r:id="rId4"/>
+    <sheet name="Q4" sheetId="5" r:id="rId5"/>
+    <sheet name="Q5" sheetId="6" r:id="rId6"/>
+    <sheet name="Q6" sheetId="7" r:id="rId7"/>
+    <sheet name="Q7" sheetId="8" r:id="rId8"/>
+    <sheet name="Q8" sheetId="9" r:id="rId9"/>
+    <sheet name="Q9" sheetId="10" r:id="rId10"/>
+    <sheet name="Q10" sheetId="11" r:id="rId11"/>
+    <sheet name="Q11" sheetId="12" r:id="rId12"/>
+    <sheet name="Q12" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="101716"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="266">
   <si>
     <t>Code</t>
   </si>
@@ -300,131 +312,545 @@
     <t>m1Ss/m2Ss/m3Ss</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Why?</t>
-  </si>
-  <si>
-    <t>m2 x 12</t>
-  </si>
-  <si>
-    <t>m2 x 8</t>
-  </si>
-  <si>
-    <t>m2 x 11</t>
-  </si>
-  <si>
-    <t>Notations used in the coding cells</t>
-  </si>
-  <si>
-    <t>m1</t>
-  </si>
-  <si>
-    <t>Student has ticked or written the answer corresponding to m1. For example, if student has ticked a=20 b=20 for q1, code is m2.</t>
-  </si>
-  <si>
-    <t>m2/m2Ss</t>
-  </si>
-  <si>
-    <t>Student has ticked or written the answer corresponding to multiple codes. For example, if student has ticked a=20 b=30 c=30 for q6, code is m2/m2Ss.</t>
-  </si>
-  <si>
-    <t>Student has ticked or written an answer for which no coding has been provided.</t>
-  </si>
-  <si>
-    <t>Student has ticked or written two different answers that correspond to 2 different codings.</t>
-  </si>
-  <si>
-    <t>Student has ticked or written one answer corresponding to m9 and one (eg a=1 b=2) for which there is no coding.</t>
-  </si>
-  <si>
-    <t>consistent if . . .</t>
-  </si>
-  <si>
-    <t>Assuming that a model such as m2 with 2 variables and its companion M2Ss with 3 variables are consistent</t>
-  </si>
-  <si>
-    <t>8 or more of the same model</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>C0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no </t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>yes (7 models in assignment)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes </t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>yes  (still in assignmnet models)</t>
-  </si>
-  <si>
-    <t>yes  (7 mod in assignment)</t>
-  </si>
-  <si>
-    <t>yes  (9 models in assignment)</t>
-  </si>
-  <si>
-    <t>Confused between m9 and m11</t>
-  </si>
-  <si>
-    <t>Confused between m8 and a unknown model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Confused between m2 and m5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(m4 to m8) x 7 </t>
-  </si>
-  <si>
-    <t>(m3 to m4) x 7</t>
-  </si>
-  <si>
-    <t>strong tendency to m2 and m10</t>
-  </si>
-  <si>
-    <t>m8 x 5   unknown model x 5</t>
-  </si>
-  <si>
-    <t>m2 x 10 + m5 x 8</t>
-  </si>
-  <si>
-    <t>strong tendency to m9</t>
-  </si>
-  <si>
-    <t>m9 x 8+</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Consistent?</t>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>20,0</t>
+  </si>
+  <si>
+    <t>20,20</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>0,10</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>10,10</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>30,20</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>30,0</t>
+  </si>
+  <si>
+    <t>10,30</t>
+  </si>
+  <si>
+    <t>0,30</t>
+  </si>
+  <si>
+    <t>10,20</t>
+  </si>
+  <si>
+    <t>20,10</t>
+  </si>
+  <si>
+    <t>20,20|10,10</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>M7</t>
+  </si>
+  <si>
+    <t>M8</t>
+  </si>
+  <si>
+    <t>M9</t>
+  </si>
+  <si>
+    <t>M11</t>
+  </si>
+  <si>
+    <t>M10</t>
+  </si>
+  <si>
+    <t>M1,S1</t>
+  </si>
+  <si>
+    <t>M1,S3|M2,S3|M3,S3|M4,S3|M11,S3</t>
+  </si>
+  <si>
+    <t>M5,S3|M6,S3|M7,S3|M2,S1</t>
+  </si>
+  <si>
+    <t>M3,S1</t>
+  </si>
+  <si>
+    <t>M4,S1</t>
+  </si>
+  <si>
+    <t>M5,S1</t>
+  </si>
+  <si>
+    <t>M6,S1</t>
+  </si>
+  <si>
+    <t>M7,S1</t>
+  </si>
+  <si>
+    <t>M8,S1</t>
+  </si>
+  <si>
+    <t>M9,S1|M11,S1|M8,S3</t>
+  </si>
+  <si>
+    <t>M10,S1|M2,S2|M4,S2</t>
+  </si>
+  <si>
+    <t>M1,S2|M3,S2</t>
+  </si>
+  <si>
+    <t>M5,S2|M7,S2</t>
+  </si>
+  <si>
+    <t>M6,S2|M8,S2</t>
+  </si>
+  <si>
+    <t>M11,S2</t>
+  </si>
+  <si>
+    <t>0,20</t>
+  </si>
+  <si>
+    <t>30,30|20,20</t>
+  </si>
+  <si>
+    <t>10,0</t>
+  </si>
+  <si>
+    <t>30,50</t>
+  </si>
+  <si>
+    <t>40,30</t>
+  </si>
+  <si>
+    <t>20,0|0,10</t>
+  </si>
+  <si>
+    <t>30,0|0,30</t>
+  </si>
+  <si>
+    <t>30,20|10,30</t>
+  </si>
+  <si>
+    <t>20,10|20,10</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>M1,S3|M2,S3|M3,S3|M4,S3</t>
+  </si>
+  <si>
+    <t>M2,S1</t>
+  </si>
+  <si>
+    <t>M5,S3|M6,S3|M7,S3|M8,S3</t>
+  </si>
+  <si>
+    <t>M9,S1|M11,S1|M11,S3</t>
+  </si>
+  <si>
+    <t>M1,S1|M3,S2</t>
+  </si>
+  <si>
+    <t>30,30</t>
+  </si>
+  <si>
+    <t>0,10|20,0</t>
+  </si>
+  <si>
+    <t>0,30|30,0</t>
+  </si>
+  <si>
+    <t>10,20|10,20</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>M2,S1|M2,S3|M1,S3</t>
+  </si>
+  <si>
+    <t>M3,S3|M4,S3|M6,S3</t>
+  </si>
+  <si>
+    <t>M5,S1|M5,S3</t>
+  </si>
+  <si>
+    <t>M7,S3|M8,S3</t>
+  </si>
+  <si>
+    <t>M9,S1</t>
+  </si>
+  <si>
+    <t>M11,S1|M11,S3</t>
+  </si>
+  <si>
+    <t>M10,S1</t>
+  </si>
+  <si>
+    <t>M1,S2</t>
+  </si>
+  <si>
+    <t>M2,S2</t>
+  </si>
+  <si>
+    <t>M3,S2</t>
+  </si>
+  <si>
+    <t>M4,S2</t>
+  </si>
+  <si>
+    <t>M5,S2</t>
+  </si>
+  <si>
+    <t>M6,S2</t>
+  </si>
+  <si>
+    <t>M7,S2</t>
+  </si>
+  <si>
+    <t>M8,S2</t>
+  </si>
+  <si>
+    <t>20,30,0</t>
+  </si>
+  <si>
+    <t>20,30,30</t>
+  </si>
+  <si>
+    <t>0,0,10</t>
+  </si>
+  <si>
+    <t>10,10,10</t>
+  </si>
+  <si>
+    <t>10,10,20</t>
+  </si>
+  <si>
+    <t>30,50,30</t>
+  </si>
+  <si>
+    <t>30,30,0</t>
+  </si>
+  <si>
+    <t>10,30,60</t>
+  </si>
+  <si>
+    <t>0,0,60</t>
+  </si>
+  <si>
+    <t>10,30,50</t>
+  </si>
+  <si>
+    <t>10,20,30</t>
+  </si>
+  <si>
+    <t>20,30,10</t>
+  </si>
+  <si>
+    <t>10,10,10|20,20,20|30,30,30</t>
+  </si>
+  <si>
+    <t>20,0,30|10,30,0</t>
+  </si>
+  <si>
+    <t>20,20,30|10,30,30</t>
+  </si>
+  <si>
+    <t>0,10,30|10,0,20</t>
+  </si>
+  <si>
+    <t>10,10,30|10,20,20</t>
+  </si>
+  <si>
+    <t>30,20,30|10,50,30</t>
+  </si>
+  <si>
+    <t>30,0,30|10,50,0</t>
+  </si>
+  <si>
+    <t>10,30,30|10,20,50</t>
+  </si>
+  <si>
+    <t>0,30,30|10,0,50</t>
+  </si>
+  <si>
+    <t>20,10,30|10,30,20</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>M1,S3|M2,S3|M11,S3</t>
+  </si>
+  <si>
+    <t>M3,S3|M4,S3</t>
+  </si>
+  <si>
+    <t>M5,S3|M6,S3</t>
+  </si>
+  <si>
+    <t>0,0,7</t>
+  </si>
+  <si>
+    <t>7,5,3</t>
+  </si>
+  <si>
+    <t>3,5,0</t>
+  </si>
+  <si>
+    <t>3,5,5</t>
+  </si>
+  <si>
+    <t>3,7,5</t>
+  </si>
+  <si>
+    <t>12,15,22</t>
+  </si>
+  <si>
+    <t>12,8,10</t>
+  </si>
+  <si>
+    <t>0,0,15</t>
+  </si>
+  <si>
+    <t>8,15,12</t>
+  </si>
+  <si>
+    <t>8,10,12</t>
+  </si>
+  <si>
+    <t>3,12,0</t>
+  </si>
+  <si>
+    <t>5,3,7</t>
+  </si>
+  <si>
+    <t>3,5,7</t>
+  </si>
+  <si>
+    <t>5,5,5|3,3,3|7,7,7</t>
+  </si>
+  <si>
+    <t>7,3,0|0,5,7|5,0,3</t>
+  </si>
+  <si>
+    <t>7,3,7|5,5,7|5,3,3</t>
+  </si>
+  <si>
+    <t>0,3,5|3,0,7|5,7,0</t>
+  </si>
+  <si>
+    <t>5,3,5|3,3,7|5,7,7</t>
+  </si>
+  <si>
+    <t>12,3,7|5,8,7|5,3,10</t>
+  </si>
+  <si>
+    <t>12,3,0|0,8,7|5,0,10</t>
+  </si>
+  <si>
+    <t>5,3,12|8,3,7|5,10,7</t>
+  </si>
+  <si>
+    <t>0,3,12|8,0,7|5,10,0</t>
+  </si>
+  <si>
+    <t>7,3,5|3,5,7|5,7,3</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>3,5,3</t>
+  </si>
+  <si>
+    <t>15,8,10</t>
+  </si>
+  <si>
+    <t>10,5,0</t>
+  </si>
+  <si>
+    <t>15,10,22</t>
+  </si>
+  <si>
+    <t>5,0,3|0,5,7|7,3,0</t>
+  </si>
+  <si>
+    <t>5,3,3|5,5,7|7,3,7</t>
+  </si>
+  <si>
+    <t>5,7,0|3,0,7|0,3,5</t>
+  </si>
+  <si>
+    <t>5,7,7|3,3,7|5,3,5</t>
+  </si>
+  <si>
+    <t>5,3,10|5,8,7|12,3,7</t>
+  </si>
+  <si>
+    <t>5,0,10|0,8,7|12,3,0</t>
+  </si>
+  <si>
+    <t>5,10,7|8,3,7|5,3,12</t>
+  </si>
+  <si>
+    <t>5,10,0|8,0,7|0,3,12</t>
+  </si>
+  <si>
+    <t>5,7,3|3,5,7|7,3,5</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>0,3,5</t>
+  </si>
+  <si>
+    <t>7,0,5</t>
+  </si>
+  <si>
+    <t>7,7,5</t>
+  </si>
+  <si>
+    <t>15,18,10</t>
+  </si>
+  <si>
+    <t>0,15,0</t>
+  </si>
+  <si>
+    <t>15,10,12</t>
+  </si>
+  <si>
+    <t>10,0,5</t>
+  </si>
+  <si>
+    <t>7,3,5</t>
+  </si>
+  <si>
+    <t>5,0,3|7,3,0|0,5,7</t>
+  </si>
+  <si>
+    <t>5,3,3|7,3,7|5,5,7</t>
+  </si>
+  <si>
+    <t>5,7,0|0,3,5|3,0,7</t>
+  </si>
+  <si>
+    <t>5,7,7|5,3,5|3,3,7</t>
+  </si>
+  <si>
+    <t>5,3,10|12,3,7|5,8,7</t>
+  </si>
+  <si>
+    <t>5,0,10|12,3,0|0,8,7</t>
+  </si>
+  <si>
+    <t>5,10,7|5,3,12|8,3,7</t>
+  </si>
+  <si>
+    <t>5,10,0|0,3,12|8,0,7</t>
+  </si>
+  <si>
+    <t>5,7,3|7,3,5|3,5,7</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>5,0,0</t>
+  </si>
+  <si>
+    <t>0,7,3</t>
+  </si>
+  <si>
+    <t>3,7,3</t>
+  </si>
+  <si>
+    <t>20,8,15</t>
+  </si>
+  <si>
+    <t>12,8,15</t>
+  </si>
+  <si>
+    <t>15,0,0</t>
+  </si>
+  <si>
+    <t>8,10,15</t>
+  </si>
+  <si>
+    <t>0,7,8</t>
+  </si>
+  <si>
+    <t>0,5,7|5,0,3|7,3,0</t>
+  </si>
+  <si>
+    <t>#11</t>
+  </si>
+  <si>
+    <t>7,5,5</t>
+  </si>
+  <si>
+    <t>0,3,0</t>
+  </si>
+  <si>
+    <t>7,0,8</t>
+  </si>
+  <si>
+    <t>8,18,15</t>
+  </si>
+  <si>
+    <t>#12</t>
+  </si>
+  <si>
+    <t>7,7,3</t>
+  </si>
+  <si>
+    <t>12,15,10</t>
+  </si>
+  <si>
+    <t>0,12,3</t>
+  </si>
+  <si>
+    <t>20,15,12</t>
+  </si>
+  <si>
+    <t>5,7,3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -474,19 +900,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -501,7 +927,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -509,7 +935,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -811,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -822,7 +1253,7 @@
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -887,7 +1318,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -952,7 +1383,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -1014,7 +1445,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -1079,7 +1510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
@@ -1144,7 +1575,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -1209,7 +1640,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>57</v>
       </c>
@@ -1274,7 +1705,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>64</v>
       </c>
@@ -1336,7 +1767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>72</v>
       </c>
@@ -1395,7 +1826,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>81</v>
       </c>
@@ -1451,7 +1882,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>82</v>
       </c>
@@ -1513,7 +1944,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
@@ -1575,7 +2006,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
@@ -1634,81 +2065,61 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="P15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="R15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="S15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="T15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="U15" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>127</v>
-      </c>
+      <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1731,74 +2142,30 @@
       <c r="U17" s="5"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="P18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q18" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="R18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="S18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="T18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>89</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -1807,43 +2174,21 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="N19" s="5" t="s">
-        <v>89</v>
-      </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-      <c r="P19" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q19" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="R19" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="S19" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="T19" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="U19" s="5" t="s">
-        <v>110</v>
-      </c>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>111</v>
-      </c>
+      <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -1855,32 +2200,18 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="N20" s="5" t="s">
-        <v>89</v>
-      </c>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
       <c r="O20" s="5"/>
-      <c r="P20" s="5" t="s">
-        <v>89</v>
-      </c>
+      <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
-      <c r="R20" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="S20" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="T20" s="5" t="s">
-        <v>89</v>
-      </c>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
       <c r="U20" s="5"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>112</v>
-      </c>
+      <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -1892,105 +2223,51 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
-      <c r="M21" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="N21" s="5" t="s">
-        <v>113</v>
-      </c>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
       <c r="O21" s="5"/>
-      <c r="P21" s="5" t="s">
-        <v>114</v>
-      </c>
+      <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
-      <c r="R21" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="S21" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="T21" s="5" t="s">
-        <v>89</v>
-      </c>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
       <c r="U21" s="5"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="A22" s="4"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>118</v>
-      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-      <c r="P22" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q22" s="3" t="s">
-        <v>120</v>
-      </c>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
-      <c r="U22" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="U22" s="3"/>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D23" s="3" t="s">
-        <v>121</v>
-      </c>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="3" t="s">
-        <v>124</v>
-      </c>
+      <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>123</v>
-      </c>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
@@ -2024,62 +2301,10 @@
       <c r="W24" s="3"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>103</v>
-      </c>
+      <c r="A27" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2087,4 +2312,2135 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
+ Sample_data.xlsx result line * results written to Sample_data_.xlsx to appropriate places
</commit_message>
<xml_diff>
--- a/data/Sample_data.xlsx
+++ b/data/Sample_data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="225">
   <si>
     <t>Code</t>
   </si>
@@ -698,6 +698,9 @@
   </si>
   <si>
     <t>7,5,3|5,3,7|7,3,5|3,7,5</t>
+  </si>
+  <si>
+    <t>Results</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1097,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1916,7 +1919,9 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
+      <c r="A14" s="5" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>

</xml_diff>